<commit_message>
Change to Alfred Implementation, Add highlighting function
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Duke Research Opportunity\Prof. Aguilar Macro Dashboard\MacroDashBoard\MacroDashboard Versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C619F0-AA12-4C13-8732-6DC9ACB4B259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE348A97-BD18-4B7F-8F45-08E626CE7546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="165">
   <si>
     <t>Present</t>
   </si>
@@ -549,6 +549,9 @@
   </si>
   <si>
     <t>DFF</t>
+  </si>
+  <si>
+    <t>Latest Period</t>
   </si>
 </sst>
 </file>
@@ -1143,22 +1146,22 @@
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="104" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43"/>
+    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="29.3984375" style="30" customWidth="1"/>
     <col min="2" max="2" width="16.265625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" style="3" customWidth="1"/>
     <col min="4" max="4" width="23.265625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.1328125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="10" width="11.1328125" style="2" customWidth="1"/>
     <col min="11" max="11" width="5.1328125" style="1" customWidth="1"/>
     <col min="12" max="12" width="26" style="30" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12" style="4" customWidth="1"/>
-    <col min="14" max="14" width="11.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.9296875" style="3" customWidth="1"/>
     <col min="15" max="15" width="21.73046875" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.1328125" style="2"/>
     <col min="17" max="21" width="11.1328125" style="2" customWidth="1"/>
@@ -1201,7 +1204,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>25</v>
@@ -1232,7 +1235,7 @@
         <v>80</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>24</v>
+        <v>164</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>25</v>
@@ -2782,7 +2785,7 @@
         <v>71</v>
       </c>
       <c r="P29" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q29" s="6">
         <v>1</v>
@@ -3413,7 +3416,7 @@
         <v>39</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q40" s="38">
         <v>1</v>

</xml_diff>

<commit_message>
Add raw table, add green highlights
</commit_message>
<xml_diff>
--- a/MacroDashboard Versions/Economic Dashboard V1-Template.xlsx
+++ b/MacroDashboard Versions/Economic Dashboard V1-Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Desktop\Duke Research Opportunity\Prof. Aguilar Macro Dashboard\MacroDashBoard\MacroDashboard Versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE348A97-BD18-4B7F-8F45-08E626CE7546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F971634-814E-4E72-9A49-FB0BFBDD9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,9 +461,6 @@
     <t>PCEPILFE</t>
   </si>
   <si>
-    <t>UMCSENT</t>
-  </si>
-  <si>
     <t>T10YIE</t>
   </si>
   <si>
@@ -509,9 +506,6 @@
     <t>CPILFESL</t>
   </si>
   <si>
-    <t>DTWEXBGS</t>
-  </si>
-  <si>
     <t>ECIWAG</t>
   </si>
   <si>
@@ -552,17 +546,24 @@
   </si>
   <si>
     <t>Latest Period</t>
+  </si>
+  <si>
+    <t>MICH</t>
+  </si>
+  <si>
+    <t>TWEXBGSMTH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="#,##0,"/>
+    <numFmt numFmtId="167" formatCode="0\%"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -716,7 +717,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -844,6 +845,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1146,8 +1150,8 @@
   </sheetPr>
   <dimension ref="A1:U80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="51" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="76" zoomScaleNormal="51" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1204,7 +1208,7 @@
         <v>80</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>25</v>
@@ -1235,7 +1239,7 @@
         <v>80</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O2" s="10" t="s">
         <v>25</v>
@@ -1503,19 +1507,19 @@
       <c r="E7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="25">
-        <v>1</v>
-      </c>
-      <c r="G7" s="25">
-        <v>1</v>
-      </c>
-      <c r="H7" s="25">
-        <v>1</v>
-      </c>
-      <c r="I7" s="25">
-        <v>1</v>
-      </c>
-      <c r="J7" s="25">
+      <c r="F7" s="44">
+        <v>1</v>
+      </c>
+      <c r="G7" s="44">
+        <v>1</v>
+      </c>
+      <c r="H7" s="44">
+        <v>1</v>
+      </c>
+      <c r="I7" s="44">
+        <v>1</v>
+      </c>
+      <c r="J7" s="44">
         <v>1</v>
       </c>
       <c r="K7" s="5"/>
@@ -1698,7 +1702,7 @@
         <v>47</v>
       </c>
       <c r="M10" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N10" s="7"/>
       <c r="O10" s="6" t="s">
@@ -1814,7 +1818,7 @@
         <v>82</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="N12" s="7"/>
       <c r="O12" s="6" t="s">
@@ -1844,7 +1848,7 @@
         <v>29</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="6" t="s">
@@ -1901,7 +1905,7 @@
     <row r="14" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A14" s="34"/>
       <c r="B14" s="15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="6" t="s">
@@ -1989,7 +1993,7 @@
         <v>84</v>
       </c>
       <c r="M15" s="15" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N15" s="7"/>
       <c r="O15" s="6" t="s">
@@ -2260,7 +2264,7 @@
         <v>23</v>
       </c>
       <c r="M20" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N20" s="7"/>
       <c r="O20" s="6" t="s">
@@ -2317,7 +2321,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="28"/>
       <c r="M21" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="N21" s="7"/>
       <c r="O21" s="6" t="s">
@@ -2721,7 +2725,7 @@
         <v>59</v>
       </c>
       <c r="M28" s="15" t="s">
-        <v>134</v>
+        <v>163</v>
       </c>
       <c r="N28" s="7"/>
       <c r="O28" s="6" t="s">
@@ -2778,7 +2782,7 @@
         <v>78</v>
       </c>
       <c r="M29" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N29" s="7"/>
       <c r="O29" s="6" t="s">
@@ -2808,7 +2812,7 @@
         <v>68</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" s="7"/>
       <c r="D30" s="6" t="s">
@@ -2837,7 +2841,7 @@
         <v>79</v>
       </c>
       <c r="M30" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N30" s="7"/>
       <c r="O30" s="6" t="s">
@@ -2865,7 +2869,7 @@
     <row r="31" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A31" s="33"/>
       <c r="B31" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="6" t="s">
@@ -2894,7 +2898,7 @@
         <v>72</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N31" s="7"/>
       <c r="O31" s="6" t="s">
@@ -2951,7 +2955,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="28"/>
       <c r="M32" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="N32" s="7"/>
       <c r="O32" s="6" t="s">
@@ -3008,7 +3012,7 @@
         <v>74</v>
       </c>
       <c r="M33" s="15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="N33" s="7"/>
       <c r="O33" s="6" t="s">
@@ -3065,7 +3069,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="28"/>
       <c r="M34" s="15" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="N34" s="7"/>
       <c r="O34" s="6" t="s">
@@ -3095,7 +3099,7 @@
         <v>83</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C35" s="7"/>
       <c r="D35" s="6" t="s">
@@ -3104,27 +3108,27 @@
       <c r="E35" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="25">
-        <v>1</v>
-      </c>
-      <c r="G35" s="25">
-        <v>1</v>
-      </c>
-      <c r="H35" s="25">
-        <v>1</v>
-      </c>
-      <c r="I35" s="25">
-        <v>1</v>
-      </c>
-      <c r="J35" s="25">
+      <c r="F35" s="44">
+        <v>1</v>
+      </c>
+      <c r="G35" s="44">
+        <v>1</v>
+      </c>
+      <c r="H35" s="44">
+        <v>1</v>
+      </c>
+      <c r="I35" s="44">
+        <v>1</v>
+      </c>
+      <c r="J35" s="44">
         <v>1</v>
       </c>
       <c r="K35" s="5"/>
       <c r="L35" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M35" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N35" s="7"/>
       <c r="O35" s="6" t="s">
@@ -3179,7 +3183,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="28"/>
       <c r="M36" s="15" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="N36" s="7"/>
       <c r="O36" s="6" t="s">
@@ -3238,7 +3242,7 @@
         <v>75</v>
       </c>
       <c r="M37" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N37" s="7"/>
       <c r="O37" s="6" t="s">
@@ -3295,7 +3299,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="28"/>
       <c r="M38" s="15" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N38" s="7"/>
       <c r="O38" s="6" t="s">
@@ -3352,14 +3356,14 @@
         <v>76</v>
       </c>
       <c r="M39" s="15" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="N39" s="7"/>
       <c r="O39" s="6" t="s">
         <v>77</v>
       </c>
       <c r="P39" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q39" s="6">
         <v>1</v>
@@ -3377,12 +3381,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:21" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A40" s="33" t="s">
         <v>66</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="6" t="s">
@@ -3409,14 +3413,14 @@
       <c r="K40" s="5"/>
       <c r="L40" s="28"/>
       <c r="M40" s="15" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="N40" s="7"/>
       <c r="O40" s="6" t="s">
         <v>39</v>
       </c>
       <c r="P40" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="Q40" s="38">
         <v>1</v>
@@ -3437,7 +3441,7 @@
     <row r="41" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A41" s="33"/>
       <c r="B41" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="6" t="s">
@@ -3466,7 +3470,7 @@
         <v>54</v>
       </c>
       <c r="M41" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N41" s="7"/>
       <c r="O41" s="6" t="s">
@@ -3496,7 +3500,7 @@
         <v>67</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="6" t="s">
@@ -3523,7 +3527,7 @@
       <c r="K42" s="7"/>
       <c r="L42" s="28"/>
       <c r="M42" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N42" s="7"/>
       <c r="O42" s="6" t="s">
@@ -3551,7 +3555,7 @@
     <row r="43" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A43" s="33"/>
       <c r="B43" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="6" t="s">
@@ -3580,7 +3584,7 @@
         <v>55</v>
       </c>
       <c r="M43" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N43" s="7"/>
       <c r="O43" s="6" t="s">
@@ -3637,7 +3641,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="28"/>
       <c r="M44" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="N44" s="7"/>
       <c r="O44" s="6" t="s">
@@ -3706,7 +3710,7 @@
         <v>33</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="6" t="s">
@@ -3765,7 +3769,7 @@
     <row r="47" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A47" s="33"/>
       <c r="B47" s="15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="6" t="s">
@@ -3794,7 +3798,7 @@
         <v>18</v>
       </c>
       <c r="M47" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="N47" s="7"/>
       <c r="O47" s="6" t="s">
@@ -3824,7 +3828,7 @@
         <v>34</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="6" t="s">
@@ -3853,7 +3857,7 @@
         <v>17</v>
       </c>
       <c r="M48" s="15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="N48" s="7"/>
       <c r="O48" s="6" t="s">
@@ -3881,7 +3885,7 @@
     <row r="49" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A49" s="33"/>
       <c r="B49" s="15" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="6" t="s">
@@ -3910,7 +3914,7 @@
         <v>19</v>
       </c>
       <c r="M49" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="N49" s="7"/>
       <c r="O49" s="6" t="s">
@@ -3940,7 +3944,7 @@
         <v>52</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="6" t="s">
@@ -3969,7 +3973,7 @@
         <v>20</v>
       </c>
       <c r="M50" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N50" s="7"/>
       <c r="O50" s="6" t="s">
@@ -3997,7 +4001,7 @@
     <row r="51" spans="1:21" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A51" s="33"/>
       <c r="B51" s="15" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C51" s="7"/>
       <c r="D51" s="6" t="s">
@@ -4026,7 +4030,7 @@
         <v>21</v>
       </c>
       <c r="M51" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N51" s="7"/>
       <c r="O51" s="6" t="s">
@@ -4067,7 +4071,7 @@
         <v>60</v>
       </c>
       <c r="M52" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="N52" s="20"/>
       <c r="O52" s="9" t="s">
@@ -4097,7 +4101,7 @@
         <v>70</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="6"/>

</xml_diff>